<commit_message>
Remove unused data files: deleted data-source-1.png and data-sources.pptx, and updated birddata_tidy.xlsx.
</commit_message>
<xml_diff>
--- a/data/birddata_tidy.xlsx
+++ b/data/birddata_tidy.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\agridat-data-services\data-HAU-bbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CE2E41D4-C510-4042-A48B-81D8C14747F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B29C80-7A39-4DCC-9AB3-027E6050782A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B8A97738-5815-4565-BAA0-82EE8530E771}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B8A97738-5815-4565-BAA0-82EE8530E771}"/>
   </bookViews>
   <sheets>
     <sheet name="birddata" sheetId="1" r:id="rId1"/>
+    <sheet name="dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3127" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3144" uniqueCount="130">
   <si>
     <t>longitude</t>
   </si>
@@ -381,13 +395,43 @@
   <si>
     <t>occasion</t>
   </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t># HAU BBS Breeding Bird Survey 2022-2024</t>
+  </si>
+  <si>
+    <t>UK vernacular common name (not international official common name)</t>
+  </si>
+  <si>
+    <t>Code containing year, transect and occasion</t>
+  </si>
+  <si>
+    <t>transect number</t>
+  </si>
+  <si>
+    <t>occasion of resampling within each transect (usually 2-3, A, B, C)</t>
+  </si>
+  <si>
+    <t>year of sample</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -869,8 +913,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1248,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C646C59C-E409-4224-A3CD-6E6640FC87AE}">
   <dimension ref="A1:G1561"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40286,4 +40330,92 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F40C19E-DE65-47CE-A07F-770859C79900}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update birddata_tidy.xlsx with new data revisions.
</commit_message>
<xml_diff>
--- a/data/birddata_tidy.xlsx
+++ b/data/birddata_tidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\agridat-data-services\data-HAU-bbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B29C80-7A39-4DCC-9AB3-027E6050782A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE99D77D-F1BB-4543-A42A-B55FA698E6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B8A97738-5815-4565-BAA0-82EE8530E771}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B8A97738-5815-4565-BAA0-82EE8530E771}"/>
   </bookViews>
   <sheets>
     <sheet name="birddata" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3144" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3146" uniqueCount="132">
   <si>
     <t>longitude</t>
   </si>
@@ -405,9 +405,6 @@
     <t># HAU BBS Breeding Bird Survey 2022-2024</t>
   </si>
   <si>
-    <t>UK vernacular common name (not international official common name)</t>
-  </si>
-  <si>
     <t>Code containing year, transect and occasion</t>
   </si>
   <si>
@@ -425,6 +422,15 @@
   <si>
     <t>lat</t>
   </si>
+  <si>
+    <t xml:space="preserve">UK vernacular common name (not international official common name, possibly adheres to BOU British List) </t>
+  </si>
+  <si>
+    <t>https://bou.org.uk/wp-content/uploads/2025/01/BOU_British_List_10th-and-57th_IOC14_2_Cat-F.pdf</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
 </sst>
 </file>
 
@@ -433,7 +439,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,6 +570,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -866,7 +880,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -909,14 +923,19 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -950,6 +969,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1292,14 +1312,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C646C59C-E409-4224-A3CD-6E6640FC87AE}">
   <dimension ref="A1:G1561"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
   </cols>
@@ -40334,88 +40353,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F40C19E-DE65-47CE-A07F-770859C79900}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{2297F774-57BC-4FEF-B2A5-4EB5B2ADCFBD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance README.md to include detailed descriptions of data files and sources, and update EDA.R script with additional analysis and visualizations for HAU BBS data.
</commit_message>
<xml_diff>
--- a/data/birddata_tidy.xlsx
+++ b/data/birddata_tidy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\agridat-data-services\data-HAU-bbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE99D77D-F1BB-4543-A42A-B55FA698E6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17BD848-E16E-4B6C-96C3-24D677CE1F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B8A97738-5815-4565-BAA0-82EE8530E771}"/>
   </bookViews>
@@ -1313,7 +1313,8 @@
   <dimension ref="A1:G1561"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A1545" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1325" sqref="A1325:XFD1325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>